<commit_message>
rough outline of a schema
</commit_message>
<xml_diff>
--- a/project/excel/pfhub_schema.xlsx
+++ b/project/excel/pfhub_schema.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dataset" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DatasetCollection" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dataset1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DatasetCollection1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Benchmark" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BenchmarkResult" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Contributor" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="File" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Implementation" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Benchmark1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="BenchmarkResult1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Contributor1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="File1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Implementation1" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,6 +422,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -439,61 +515,27 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>contributors</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Dataset_primary_email</t>
+          <t>benchmark</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>framework</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>hardware</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>datasetCollection__entries</t>
+          <t>implementation</t>
         </is>
       </c>
     </row>
@@ -508,6 +550,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>handle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>affiliation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -529,16 +617,88 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -565,62 +725,82 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>contributors</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Dataset_primary_email</t>
+          <t>benchmark</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>framework</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>hardware</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>datasetCollection__entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>implementation</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>handle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>affiliation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -647,7 +827,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>format</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Detailed PFHub schema implementation.
</commit_message>
<xml_diff>
--- a/project/excel/pfhub_schema.xlsx
+++ b/project/excel/pfhub_schema.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="15" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Benchmark" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="BenchmarkResult" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Contributor" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="File" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Implementation" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Benchmark1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="BenchmarkResult1" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Contributor1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="File1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Implementation1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Benchmark" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchmarkResult" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ComputeResource" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contributor" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="File" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Software" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SourceCode" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Benchmark1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchmarkResult1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ComputeResource1" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contributor1" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="File1" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Software1" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SourceCode1" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -422,6 +428,108 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contributors</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>benchmark</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>framework</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>implementation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>results</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -433,6 +541,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>architecture</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>cores</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nodes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -443,6 +587,154 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>handle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>affiliation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>columns</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>data_raw</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data_table</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>data_visualization</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>hardware</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>memory_in_KB</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>time_in_s</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>download</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>repository</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>version</t>
         </is>
       </c>
@@ -452,7 +744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -494,7 +786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,21 +822,200 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>implementation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>results</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>summary</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>architecture</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>cores</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nodes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>handle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>affiliation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>columns</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>data_raw</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data_table</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>data_visualization</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>hardware</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>implementation</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>memory_in_KB</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>time_in_s</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -571,26 +1042,26 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>handle</t>
+          <t>download</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>affiliation</t>
+          <t>repository</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>email</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -617,22 +1088,22 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>format</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
+          <t>repository</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,41 +1124,10 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>repository</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>number</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
@@ -696,142 +1136,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>contributors</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>benchmark</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>framework</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>hardware</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>implementation</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>handle</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>affiliation</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update fields for MOOSE example.
</commit_message>
<xml_diff>
--- a/project/excel/pfhub_schema.xlsx
+++ b/project/excel/pfhub_schema.xlsx
@@ -1,32 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="19" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="21" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BenchmarkResult" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ComputeResource" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Contributor" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="CsvFile" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="DataFile" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="File" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Results" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Software" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="SourceCode" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="VisualizationFile" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="BenchmarkResult1" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="ComputeResource1" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Contributor1" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="CsvFile1" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="DataFile1" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="File2" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Results1" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Software1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="SourceCode1" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="VisualizationFile1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchmarkResult" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ComputeResource" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contributor" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CsvFile" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataFile" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="File" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Software" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SourceCode" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarball" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VisualizationFile" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BenchmarkResult1" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ComputeResource1" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contributor1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CsvFile1" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataFile1" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="File2" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results1" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Software1" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SourceCode1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarball1" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VisualizationFile1" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -522,6 +524,45 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Tarball_format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"tgz,tar.gz"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"tgz,tar.gz"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>File_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>format</t>
         </is>
       </c>
@@ -531,7 +572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -597,7 +638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -633,7 +674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -679,7 +720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -701,21 +742,404 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>columns</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>CsvFile_format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>File_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>format</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>File_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>csv_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>raw_data</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>viz_data</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>hardware</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>memory_in_kb</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>time_in_s</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Software_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>commit</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>download</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>architecture</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>cores</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nodes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SourceCode_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>commit</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>File_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tarball_format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>File_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>handle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>affiliation</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>File_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>columns</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>CsvFile_format</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"csv"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"csv"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -746,7 +1170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -777,7 +1201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -828,7 +1252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -855,14 +1279,14 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>commit</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>download</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>repository</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
           <t>version</t>
@@ -874,7 +1298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -901,351 +1325,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>repository</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>architecture</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>cores</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nodes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>File_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>handle</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>affiliation</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>File_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>columns</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>File_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>File_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>csv_data</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>raw_data</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>viz_data</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>hardware</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>memory_in_kb</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>time_in_s</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Software_url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>download</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>repository</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>SourceCode_url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>repository</t>
+          <t>commit</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add schema field to schema definitions.
</commit_message>
<xml_diff>
--- a/project/excel/pfhub_schema.xlsx
+++ b/project/excel/pfhub_schema.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
         </is>
       </c>
       <c r="I1" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>summary</t>
         </is>
@@ -492,10 +497,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"1a,1b,1c,1d"</formula1>
+      <formula1>"1a,1b,1c,1d,2a,2b,2c,2d,3a,4a,4b,4c,4d,4e,4f,4g,4h,5a,5b,6a,6b,7a,7b,7c,8a,8b,8c"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"1a,1b,1c,1d"</formula1>
+      <formula1>"1a,1b,1c,1d,2a,2b,2c,2d,3a,4a,4b,4c,4d,4e,4f,4g,4h,5a,5b,6a,6b,7a,7b,7c,8a,8b,8c"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -578,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,6 +633,11 @@
         </is>
       </c>
       <c r="I1" t="inlineStr">
+        <is>
+          <t>schema</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>summary</t>
         </is>

</xml_diff>

<commit_message>
Add fictive time to schema.
</commit_message>
<xml_diff>
--- a/project/excel/pfhub_schema.xlsx
+++ b/project/excel/pfhub_schema.xlsx
@@ -834,7 +834,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -860,15 +860,20 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>fictive_time</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>hardware</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>memory_in_kb</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>time_in_s</t>
         </is>
@@ -1217,7 +1222,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1243,43 +1248,94 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>fictive_time</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>hardware</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>memory_in_kb</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>time_in_s</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Software_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>commit</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>download</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>memory_in_kb</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>time_in_s</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Software_url</t>
+          <t>version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SourceCode_url</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1292,52 +1348,6 @@
           <t>commit</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>download</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>SourceCode_url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>commit</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>